<commit_message>
Visualization and output of pred_onsets and pred_rates for Partial trials of SST data. Saved arrays of model predicted values.
</commit_message>
<xml_diff>
--- a/Working/GS_comparisons_exp_vs_predicted.xlsx
+++ b/Working/GS_comparisons_exp_vs_predicted.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="324" windowWidth="19416" windowHeight="9276"/>
+    <workbookView xWindow="288" yWindow="324" windowWidth="18936" windowHeight="7176" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="onset_times" sheetId="1" r:id="rId1"/>
     <sheet name="onset_rates" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="SST_onset_times" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>exp onsets</t>
   </si>
@@ -153,6 +153,24 @@
   <si>
     <t>experiment av</t>
   </si>
+  <si>
+    <t>Predicted</t>
+  </si>
+  <si>
+    <t>Simulated from experimental averages &amp; sd</t>
+  </si>
+  <si>
+    <t>Partial</t>
+  </si>
+  <si>
+    <t>2 sample, equal variance</t>
+  </si>
+  <si>
+    <t>2 sample, unequal variance</t>
+  </si>
+  <si>
+    <t>paired</t>
+  </si>
 </sst>
 </file>
 
@@ -199,7 +217,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +233,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -345,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -364,6 +388,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,7 +685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M374"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -6030,12 +6055,1429 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F173"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.22699999999999901</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.12927116194649199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="B3" s="1">
+        <v>5.89999999999999E-2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.187058396956511</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="B4" s="1">
+        <v>0.157</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.28753523759994298</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="B5" s="1">
+        <v>0.181999999999999</v>
+      </c>
+      <c r="C5" s="1">
+        <v>8.2103384209805202E-2</v>
+      </c>
+      <c r="E5">
+        <f>TTEST(B2:B173,C2:C173,2,1)</f>
+        <v>0.90912954186635142</v>
+      </c>
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="B6" s="1">
+        <v>0.19799999999999901</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.12787707749386901</v>
+      </c>
+      <c r="E6" s="18">
+        <f>TTEST(B2:B173,C2:C173,2,2)</f>
+        <v>0.9067567906372016</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7" s="1">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.22274417786342901</v>
+      </c>
+      <c r="E7">
+        <f>TTEST(B2:B173,C2:C173,2,3)</f>
+        <v>0.90675743629419725</v>
+      </c>
+      <c r="F7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" s="1">
+        <v>0.11599999999999901</v>
+      </c>
+      <c r="C8" s="1">
+        <v>8.9255299513187794E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" s="1">
+        <v>4.0999999999999898E-2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8.51722235614428E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10" s="1">
+        <v>0.122999999999999</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.23749698221122501</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11" s="1">
+        <v>0.103999999999999</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.15575355383109299</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="B12" s="1">
+        <v>-1.7999999999999999E-2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.10072900195800601</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" s="1">
+        <v>0.161</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.14190781259122801</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14" s="1">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.258873514244648</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15" s="1">
+        <v>5.4999999999999903E-2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.152391145635521</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="B16" s="1">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="C16" s="1">
+        <v>-4.1827618132776398E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="1">
+        <v>8.1999999999999906E-2</v>
+      </c>
+      <c r="C17" s="1">
+        <v>6.4266110942602303E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="1">
+        <v>2.5999999999999902E-2</v>
+      </c>
+      <c r="C18" s="1">
+        <v>7.5498590203786894E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" s="1">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.30059469641533798</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" s="1">
+        <v>0.119999999999999</v>
+      </c>
+      <c r="C20" s="1">
+        <v>4.6348360271525599E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" s="1">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.14180357542272801</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" s="1">
+        <v>0.24199999999999899</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.16504736269430301</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" s="1">
+        <v>0.113999999999999</v>
+      </c>
+      <c r="C23" s="1">
+        <v>8.0373608847754102E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" s="1">
+        <v>0.23499999999999899</v>
+      </c>
+      <c r="C24" s="1">
+        <v>5.5124677595349697E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" s="1">
+        <v>8.2999999999999893E-2</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.130587420516484</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" s="1">
+        <v>0.191999999999999</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.28424115539342898</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" s="1">
+        <v>0.19799999999999901</v>
+      </c>
+      <c r="C27" s="1">
+        <v>5.5589819600023703E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="B28" s="1">
+        <v>0.108999999999999</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.109067224822591</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3">
+      <c r="B29" s="1">
+        <v>0.213999999999999</v>
+      </c>
+      <c r="C29" s="1">
+        <v>4.75431386405505E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" s="1">
+        <v>2.5999999999999902E-2</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.21172341499450301</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" s="1">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.159220119098538</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="B32" s="1">
+        <v>0.158</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.21620252212438801</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33" s="1">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.22151013843842199</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34" s="1">
+        <v>-4.8000000000000001E-2</v>
+      </c>
+      <c r="C34" s="1">
+        <v>6.6810106328265895E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="1">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2.8569654169397898E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3">
+      <c r="B36" s="1">
+        <v>0.108999999999999</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0.175139644929341</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0.124903894455105</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38" s="1">
+        <v>9.5999999999999905E-2</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0.14563997710125601</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="B39" s="1">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0.141119769387025</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40" s="1">
+        <v>0.247999999999999</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0.13900578049543899</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="B41" s="1">
+        <v>8.0999999999999905E-2</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0.16145559148920599</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3">
+      <c r="B42" s="1">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="C42" s="1">
+        <v>9.9742738950456794E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3">
+      <c r="B43" s="1">
+        <v>-7.0999999999999994E-2</v>
+      </c>
+      <c r="C43" s="1">
+        <v>0.15922865163659</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3">
+      <c r="B44" s="1">
+        <v>0.183999999999999</v>
+      </c>
+      <c r="C44" s="1">
+        <v>-4.11929212960832E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3">
+      <c r="B45" s="1">
+        <v>0.191999999999999</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0.16846186674777</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3">
+      <c r="B46" s="1">
+        <v>0.214999999999999</v>
+      </c>
+      <c r="C46" s="1">
+        <v>4.7567010980336097E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3">
+      <c r="B47" s="1">
+        <v>0.154</v>
+      </c>
+      <c r="C47" s="1">
+        <v>9.5767823121547094E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3">
+      <c r="B48" s="1">
+        <v>0.217999999999999</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0.18494861798420401</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49" s="1">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0.20129441920361099</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3">
+      <c r="B50" s="1">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0.14048086380400501</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3">
+      <c r="B51" s="1">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="C51" s="1">
+        <v>4.3906903289262098E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3">
+      <c r="B52" s="1">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="C52" s="1">
+        <v>4.9179120194237397E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3">
+      <c r="B53" s="1">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0.156528570394524</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3">
+      <c r="B54" s="1">
+        <v>0.157</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0.197824917848896</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3">
+      <c r="B55" s="1">
+        <v>9.4999999999999904E-2</v>
+      </c>
+      <c r="C55" s="1">
+        <v>0.194351892729378</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3">
+      <c r="B56" s="1">
+        <v>0.17799999999999899</v>
+      </c>
+      <c r="C56" s="1">
+        <v>8.7729896557019502E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3">
+      <c r="B57" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C57" s="1">
+        <v>0.173186573683657</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3">
+      <c r="B58" s="1">
+        <v>1.6999999999999901E-2</v>
+      </c>
+      <c r="C58" s="1">
+        <v>0.103831776697924</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3">
+      <c r="B59" s="1">
+        <v>9.09999999999999E-2</v>
+      </c>
+      <c r="C59" s="1">
+        <v>0.18156271818945</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3">
+      <c r="B60" s="1">
+        <v>0.11699999999999899</v>
+      </c>
+      <c r="C60" s="1">
+        <v>0.18616101987877101</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3">
+      <c r="B61" s="1">
+        <v>0.189999999999999</v>
+      </c>
+      <c r="C61" s="1">
+        <v>0.22987008640401299</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3">
+      <c r="B62" s="1">
+        <v>0.217999999999999</v>
+      </c>
+      <c r="C62" s="1">
+        <v>9.3926784560929205E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3">
+      <c r="B63" s="1">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="C63" s="1">
+        <v>0.18245443232813599</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3">
+      <c r="B64" s="1">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="C64" s="1">
+        <v>0.15570605334068399</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3">
+      <c r="B65" s="1">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="C65" s="1">
+        <v>0.11547976580017399</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3">
+      <c r="B66" s="1">
+        <v>0.10099999999999899</v>
+      </c>
+      <c r="C66" s="1">
+        <v>0.190143079816843</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3">
+      <c r="B67" s="1">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="C67" s="1">
+        <v>0.106786984895042</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3">
+      <c r="B68" s="1">
+        <v>0.20699999999999899</v>
+      </c>
+      <c r="C68" s="1">
+        <v>0.137382609411134</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3">
+      <c r="B69" s="1">
+        <v>3.9999999999999897E-2</v>
+      </c>
+      <c r="C69" s="1">
+        <v>0.20223793166929999</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3">
+      <c r="B70" s="1">
+        <v>0.252</v>
+      </c>
+      <c r="C70" s="1">
+        <v>0.123021133415275</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3">
+      <c r="B71" s="1">
+        <v>0.19399999999999901</v>
+      </c>
+      <c r="C71" s="1">
+        <v>0.108785554745366</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3">
+      <c r="B72" s="1">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="C72" s="1">
+        <v>0.13770069261002399</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3">
+      <c r="B73" s="1">
+        <v>0.23699999999999899</v>
+      </c>
+      <c r="C73" s="1">
+        <v>4.4505459762946703E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3">
+      <c r="B74" s="1">
+        <v>0.23799999999999899</v>
+      </c>
+      <c r="C74" s="1">
+        <v>3.2588747498105098E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3">
+      <c r="B75" s="1">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="C75" s="1">
+        <v>6.1448032233596198E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3">
+      <c r="B76" s="1">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="C76" s="1">
+        <v>7.1165914153513796E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3">
+      <c r="B77" s="1">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="C77" s="1">
+        <v>5.4613443992907601E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3">
+      <c r="B78" s="1">
+        <v>3.4999999999999899E-2</v>
+      </c>
+      <c r="C78" s="1">
+        <v>0.183104124517251</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3">
+      <c r="B79" s="1">
+        <v>9.1999999999999901E-2</v>
+      </c>
+      <c r="C79" s="1">
+        <v>0.235273702035451</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3">
+      <c r="B80" s="1">
+        <v>0.190999999999999</v>
+      </c>
+      <c r="C80" s="1">
+        <v>0.16553358802134299</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3">
+      <c r="B81" s="1">
+        <v>0.19499999999999901</v>
+      </c>
+      <c r="C81" s="1">
+        <v>0.170368871807907</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3">
+      <c r="B82" s="1">
+        <v>0.20299999999999899</v>
+      </c>
+      <c r="C82" s="1">
+        <v>0.10974488779273001</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3">
+      <c r="B83" s="1">
+        <v>0.23099999999999901</v>
+      </c>
+      <c r="C83" s="1">
+        <v>0.22285145120022201</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3">
+      <c r="B84" s="1">
+        <v>6.1999999999999902E-2</v>
+      </c>
+      <c r="C84" s="1">
+        <v>0.119514292073096</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3">
+      <c r="B85" s="1">
+        <v>8.7999999999999898E-2</v>
+      </c>
+      <c r="C85" s="1">
+        <v>4.4756544330589697E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3">
+      <c r="B86" s="1">
+        <v>9.5999999999999905E-2</v>
+      </c>
+      <c r="C86" s="1">
+        <v>0.188481667596897</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3">
+      <c r="B87" s="1">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="C87" s="1">
+        <v>0.241569070847753</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3">
+      <c r="B88" s="1">
+        <v>5.9999999999999901E-2</v>
+      </c>
+      <c r="C88" s="1">
+        <v>0.15515310611343</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3">
+      <c r="B89" s="1">
+        <v>9.6999999999999906E-2</v>
+      </c>
+      <c r="C89" s="1">
+        <v>0.20104726877442899</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3">
+      <c r="B90" s="1">
+        <v>0.112999999999999</v>
+      </c>
+      <c r="C90" s="1">
+        <v>7.5280453912388703E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3">
+      <c r="B91" s="1">
+        <v>0.154</v>
+      </c>
+      <c r="C91" s="1">
+        <v>0.198564771668509</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3">
+      <c r="B92" s="1">
+        <v>0.151</v>
+      </c>
+      <c r="C92" s="1">
+        <v>0.14674639123091399</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3">
+      <c r="B93" s="1">
+        <v>5.6999999999999898E-2</v>
+      </c>
+      <c r="C93" s="1">
+        <v>0.25372283717972299</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3">
+      <c r="B94" s="1">
+        <v>0.108999999999999</v>
+      </c>
+      <c r="C94" s="1">
+        <v>0.23081737127281199</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3">
+      <c r="B95" s="1">
+        <v>0.108999999999999</v>
+      </c>
+      <c r="C95" s="1">
+        <v>8.5492750322877606E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3">
+      <c r="B96" s="1">
+        <v>0.104999999999999</v>
+      </c>
+      <c r="C96" s="1">
+        <v>0.193596129538992</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3">
+      <c r="B97" s="1">
+        <v>0.11599999999999901</v>
+      </c>
+      <c r="C97" s="1">
+        <v>9.9302425395337499E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3">
+      <c r="B98" s="1">
+        <v>0.123999999999999</v>
+      </c>
+      <c r="C98" s="1">
+        <v>0.13148158135010399</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3">
+      <c r="B99" s="1">
+        <v>0.122999999999999</v>
+      </c>
+      <c r="C99" s="1">
+        <v>0.16665883991076599</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3">
+      <c r="B100" s="1">
+        <v>0.23599999999999899</v>
+      </c>
+      <c r="C100" s="1">
+        <v>0.17149712041481499</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3">
+      <c r="B101" s="1">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="C101" s="1">
+        <v>0.24898993324669499</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3">
+      <c r="B102" s="1">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="C102" s="1">
+        <v>0.18237351329599499</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3">
+      <c r="B103" s="1">
+        <v>0.20299999999999899</v>
+      </c>
+      <c r="C103" s="1">
+        <v>-1.7027769346870301E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3">
+      <c r="B104" s="1">
+        <v>0.128</v>
+      </c>
+      <c r="C104" s="1">
+        <v>1.04563587847141E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3">
+      <c r="B105" s="1">
+        <v>8.2999999999999893E-2</v>
+      </c>
+      <c r="C105" s="1">
+        <v>0.29345798055401601</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3">
+      <c r="B106" s="1">
+        <v>0.187999999999999</v>
+      </c>
+      <c r="C106" s="1">
+        <v>9.9750331844089601E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3">
+      <c r="B107" s="1">
+        <v>0.21199999999999899</v>
+      </c>
+      <c r="C107" s="1">
+        <v>0.20483777157954899</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3">
+      <c r="B108" s="1">
+        <v>0.112999999999999</v>
+      </c>
+      <c r="C108" s="1">
+        <v>0.189610717169858</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3">
+      <c r="B109" s="1">
+        <v>0.191999999999999</v>
+      </c>
+      <c r="C109" s="1">
+        <v>4.3964870850361402E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3">
+      <c r="B110" s="1">
+        <v>0.19799999999999901</v>
+      </c>
+      <c r="C110" s="1">
+        <v>0.11817496048170199</v>
+      </c>
+    </row>
+    <row r="111" spans="2:3">
+      <c r="B111" s="1">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="C111" s="1">
+        <v>3.6256249053397603E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3">
+      <c r="B112" s="1">
+        <v>3.7999999999999902E-2</v>
+      </c>
+      <c r="C112" s="1">
+        <v>0.25215361754979199</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3">
+      <c r="B113" s="1">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="C113" s="1">
+        <v>0.13551862569404</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3">
+      <c r="B114" s="1">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="C114" s="1">
+        <v>0.37870777829139202</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3">
+      <c r="B115" s="1">
+        <v>0.305999999999999</v>
+      </c>
+      <c r="C115" s="1">
+        <v>0.211043808824246</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3">
+      <c r="B116" s="1">
+        <v>0.20399999999999899</v>
+      </c>
+      <c r="C116" s="1">
+        <v>0.21575629730583401</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3">
+      <c r="B117" s="1">
+        <v>8.99999999999999E-2</v>
+      </c>
+      <c r="C117" s="1">
+        <v>0.132853466968087</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3">
+      <c r="B118" s="1">
+        <v>9.4999999999999904E-2</v>
+      </c>
+      <c r="C118" s="1">
+        <v>0.17270188275958101</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3">
+      <c r="B119" s="1">
+        <v>0.188999999999999</v>
+      </c>
+      <c r="C119" s="1">
+        <v>0.198493135797011</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3">
+      <c r="B120" s="1">
+        <v>0.20799999999999899</v>
+      </c>
+      <c r="C120" s="1">
+        <v>0.206561268746279</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3">
+      <c r="B121" s="1">
+        <v>8.0999999999999905E-2</v>
+      </c>
+      <c r="C121" s="1">
+        <v>0.260489703471317</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3">
+      <c r="B122" s="1">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="C122" s="1">
+        <v>0.219352140313369</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3">
+      <c r="B123" s="1">
+        <v>0.22899999999999901</v>
+      </c>
+      <c r="C123" s="1">
+        <v>0.18223100322435301</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3">
+      <c r="B124" s="1">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="C124" s="1">
+        <v>-1.7847753645694399E-3</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3">
+      <c r="B125" s="1">
+        <v>0.215999999999999</v>
+      </c>
+      <c r="C125" s="1">
+        <v>0.15300475421933499</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3">
+      <c r="B126" s="1">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="C126" s="1">
+        <v>0.25261274311190901</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3">
+      <c r="B127" s="1">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="C127" s="1">
+        <v>0.227769228371522</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3">
+      <c r="B128" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="C128" s="1">
+        <v>0.174102454797918</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3">
+      <c r="B129" s="1">
+        <v>0.212999999999999</v>
+      </c>
+      <c r="C129" s="1">
+        <v>3.90793912258647E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3">
+      <c r="B130" s="1">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="C130" s="1">
+        <v>0.100881941399715</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3">
+      <c r="B131" s="1">
+        <v>0.11499999999999901</v>
+      </c>
+      <c r="C131" s="1">
+        <v>0.13463175882984099</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3">
+      <c r="B132" s="1">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="C132" s="1">
+        <v>0.29554059845949099</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3">
+      <c r="B133" s="1">
+        <v>0.191999999999999</v>
+      </c>
+      <c r="C133" s="1">
+        <v>5.7560297228074903E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3">
+      <c r="B134" s="1">
+        <v>0.23099999999999901</v>
+      </c>
+      <c r="C134" s="1">
+        <v>0.13519051775419799</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3">
+      <c r="B135" s="1">
+        <v>0.159</v>
+      </c>
+      <c r="C135" s="1">
+        <v>9.7106623106507695E-2</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3">
+      <c r="B136" s="1">
+        <v>5.4999999999999903E-2</v>
+      </c>
+      <c r="C136" s="1">
+        <v>0.222049693554704</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3">
+      <c r="B137" s="1">
+        <v>0.187999999999999</v>
+      </c>
+      <c r="C137" s="1">
+        <v>3.9861012536288001E-2</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3">
+      <c r="B138" s="1">
+        <v>5.9999999999999901E-2</v>
+      </c>
+      <c r="C138" s="1">
+        <v>3.7574488938582701E-2</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3">
+      <c r="B139" s="1">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="C139" s="1">
+        <v>1.5109923159178199E-2</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3">
+      <c r="B140" s="1">
+        <v>0.251</v>
+      </c>
+      <c r="C140" s="1">
+        <v>0.17218032251475701</v>
+      </c>
+    </row>
+    <row r="141" spans="2:3">
+      <c r="B141" s="1">
+        <v>0.217999999999999</v>
+      </c>
+      <c r="C141" s="1">
+        <v>0.19053985178629501</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3">
+      <c r="B142" s="1">
+        <v>0.20899999999999899</v>
+      </c>
+      <c r="C142" s="1">
+        <v>0.15219829384049699</v>
+      </c>
+    </row>
+    <row r="143" spans="2:3">
+      <c r="B143" s="1">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="C143" s="1">
+        <v>9.9216645685930596E-2</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3">
+      <c r="B144" s="1">
+        <v>0.23499999999999899</v>
+      </c>
+      <c r="C144" s="1">
+        <v>4.1253808378586498E-2</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3">
+      <c r="B145" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="C145" s="1">
+        <v>0.32662434754548397</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3">
+      <c r="B146" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C146" s="1">
+        <v>5.8629586279812997E-2</v>
+      </c>
+    </row>
+    <row r="147" spans="2:3">
+      <c r="B147" s="1">
+        <v>0.113999999999999</v>
+      </c>
+      <c r="C147" s="1">
+        <v>7.9517673197525604E-2</v>
+      </c>
+    </row>
+    <row r="148" spans="2:3">
+      <c r="B148" s="1">
+        <v>5.3999999999999902E-2</v>
+      </c>
+      <c r="C148" s="1">
+        <v>5.0417550550924797E-2</v>
+      </c>
+    </row>
+    <row r="149" spans="2:3">
+      <c r="B149" s="1">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="C149" s="1">
+        <v>2.85744464111958E-2</v>
+      </c>
+    </row>
+    <row r="150" spans="2:3">
+      <c r="B150" s="1">
+        <v>0.161</v>
+      </c>
+      <c r="C150" s="1">
+        <v>0.126096152986268</v>
+      </c>
+    </row>
+    <row r="151" spans="2:3">
+      <c r="B151" s="1">
+        <v>0.215999999999999</v>
+      </c>
+      <c r="C151" s="1">
+        <v>8.7582024169224601E-2</v>
+      </c>
+    </row>
+    <row r="152" spans="2:3">
+      <c r="B152" s="1">
+        <v>0.120999999999999</v>
+      </c>
+      <c r="C152" s="1">
+        <v>5.9100939245992599E-2</v>
+      </c>
+    </row>
+    <row r="153" spans="2:3">
+      <c r="B153" s="1">
+        <v>0.20799999999999899</v>
+      </c>
+      <c r="C153" s="1">
+        <v>0.24959048062167499</v>
+      </c>
+    </row>
+    <row r="154" spans="2:3">
+      <c r="B154" s="1">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C154" s="1">
+        <v>0.153516704172174</v>
+      </c>
+    </row>
+    <row r="155" spans="2:3">
+      <c r="B155" s="1">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="C155" s="1">
+        <v>5.79610384692478E-2</v>
+      </c>
+    </row>
+    <row r="156" spans="2:3">
+      <c r="B156" s="1">
+        <v>3.8999999999999903E-2</v>
+      </c>
+      <c r="C156" s="1">
+        <v>7.0879982208500697E-2</v>
+      </c>
+    </row>
+    <row r="157" spans="2:3">
+      <c r="B157" s="1">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C157" s="1">
+        <v>0.154305689150328</v>
+      </c>
+    </row>
+    <row r="158" spans="2:3">
+      <c r="B158" s="1">
+        <v>0.128</v>
+      </c>
+      <c r="C158" s="1">
+        <v>0.12918484912178799</v>
+      </c>
+    </row>
+    <row r="159" spans="2:3">
+      <c r="B159" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="C159" s="1">
+        <v>0.19226924869898501</v>
+      </c>
+    </row>
+    <row r="160" spans="2:3">
+      <c r="B160" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="C160" s="1">
+        <v>0.133226495722715</v>
+      </c>
+    </row>
+    <row r="161" spans="2:3">
+      <c r="B161" s="1">
+        <v>5.19999999999999E-2</v>
+      </c>
+      <c r="C161" s="1">
+        <v>6.26347862752729E-2</v>
+      </c>
+    </row>
+    <row r="162" spans="2:3">
+      <c r="B162" s="1">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="C162" s="1">
+        <v>0.19976884846774601</v>
+      </c>
+    </row>
+    <row r="163" spans="2:3">
+      <c r="B163" s="1">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="C163" s="1">
+        <v>7.8504287793031105E-2</v>
+      </c>
+    </row>
+    <row r="164" spans="2:3">
+      <c r="B164" s="1">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="C164" s="1">
+        <v>0.14118184658748301</v>
+      </c>
+    </row>
+    <row r="165" spans="2:3">
+      <c r="B165" s="1">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="C165" s="1">
+        <v>0.11740166412530501</v>
+      </c>
+    </row>
+    <row r="166" spans="2:3">
+      <c r="B166" s="1">
+        <v>0.11699999999999899</v>
+      </c>
+      <c r="C166" s="1">
+        <v>0.20252603834152</v>
+      </c>
+    </row>
+    <row r="167" spans="2:3">
+      <c r="B167" s="1">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="C167" s="1">
+        <v>0.15611728008546399</v>
+      </c>
+    </row>
+    <row r="168" spans="2:3">
+      <c r="B168" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C168" s="1">
+        <v>0.14791072914668299</v>
+      </c>
+    </row>
+    <row r="169" spans="2:3">
+      <c r="B169" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="C169" s="1">
+        <v>0.188425523325112</v>
+      </c>
+    </row>
+    <row r="170" spans="2:3">
+      <c r="B170" s="1">
+        <v>0.161</v>
+      </c>
+      <c r="C170" s="1">
+        <v>-3.1108985418111398E-2</v>
+      </c>
+    </row>
+    <row r="171" spans="2:3">
+      <c r="B171" s="1">
+        <v>9.8999999999999894E-2</v>
+      </c>
+      <c r="C171" s="1">
+        <v>0.22356138277149301</v>
+      </c>
+    </row>
+    <row r="172" spans="2:3">
+      <c r="B172" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="C172" s="1">
+        <v>0.14751078751479099</v>
+      </c>
+    </row>
+    <row r="173" spans="2:3">
+      <c r="B173" s="1">
+        <v>0.127</v>
+      </c>
+      <c r="C173" s="1">
+        <v>0.117287311589392</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Changed underlying Go curve function to simple Gaussian. Calculated EMG offsets from experimental data for each participant. Calculated average burst duration as 107 ms, added 107ms to each EMG onset time in data_onsets in code.
</commit_message>
<xml_diff>
--- a/Working/GS_comparisons_exp_vs_predicted.xlsx
+++ b/Working/GS_comparisons_exp_vs_predicted.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t>exp onsets</t>
   </si>
@@ -170,6 +170,18 @@
   </si>
   <si>
     <t>paired</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>predicted</t>
+  </si>
+  <si>
+    <t>i.e. 539ms after Go signal (400 plus 139ms)</t>
   </si>
 </sst>
 </file>
@@ -6055,18 +6067,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F173"/>
+  <dimension ref="A1:G173"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -6077,7 +6090,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -6088,7 +6101,7 @@
         <v>0.12927116194649199</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="B3" s="1">
         <v>5.89999999999999E-2</v>
       </c>
@@ -6096,7 +6109,7 @@
         <v>0.187058396956511</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="B4" s="1">
         <v>0.157</v>
       </c>
@@ -6104,7 +6117,7 @@
         <v>0.28753523759994298</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="B5" s="1">
         <v>0.181999999999999</v>
       </c>
@@ -6119,7 +6132,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="B6" s="1">
         <v>0.19799999999999901</v>
       </c>
@@ -6134,7 +6147,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="B7" s="1">
         <v>0.13600000000000001</v>
       </c>
@@ -6149,7 +6162,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="B8" s="1">
         <v>0.11599999999999901</v>
       </c>
@@ -6157,31 +6170,51 @@
         <v>8.9255299513187794E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="B9" s="1">
         <v>4.0999999999999898E-2</v>
       </c>
       <c r="C9" s="1">
         <v>8.51722235614428E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="B10" s="1">
         <v>0.122999999999999</v>
       </c>
       <c r="C10" s="1">
         <v>0.23749698221122501</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="1">
+        <f>AVERAGE(B2:B173)</f>
+        <v>0.13934302325581352</v>
+      </c>
+      <c r="G10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="B11" s="1">
         <v>0.103999999999999</v>
       </c>
       <c r="C11" s="1">
         <v>0.15575355383109299</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="E11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11">
+        <f>STDEV(B2:B173)</f>
+        <v>6.9030917796731373E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="B12" s="1">
         <v>-1.7999999999999999E-2</v>
       </c>
@@ -6189,7 +6222,7 @@
         <v>0.10072900195800601</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:7">
       <c r="B13" s="1">
         <v>0.161</v>
       </c>
@@ -6197,7 +6230,7 @@
         <v>0.14190781259122801</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:7">
       <c r="B14" s="1">
         <v>0.13700000000000001</v>
       </c>
@@ -6205,7 +6238,7 @@
         <v>0.258873514244648</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:7">
       <c r="B15" s="1">
         <v>5.4999999999999903E-2</v>
       </c>
@@ -6213,7 +6246,7 @@
         <v>0.152391145635521</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7">
       <c r="B16" s="1">
         <v>0.13600000000000001</v>
       </c>

</xml_diff>